<commit_message>
ERV And ARS constraints added
</commit_message>
<xml_diff>
--- a/ExcelReading/inputResources/ConstraintsToJSON.xlsx
+++ b/ExcelReading/inputResources/ConstraintsToJSON.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CodeBase\excelTojson\ExcelToJSON\ExcelReading\inputResources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3ABF67E-CC0A-47C7-AC11-A1352FCB26FD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B31C5120-54E8-4DA7-BE52-DE6C50C10DB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{1F0430CC-FF32-404D-8E6F-02861FD37FCA}"/>
+    <workbookView xWindow="2160" yWindow="2160" windowWidth="17280" windowHeight="8964" firstSheet="2" activeTab="7" xr2:uid="{1F0430CC-FF32-404D-8E6F-02861FD37FCA}"/>
   </bookViews>
   <sheets>
     <sheet name="PDU" sheetId="1" r:id="rId1"/>
@@ -20,15 +15,17 @@
     <sheet name="Rack" sheetId="11" r:id="rId5"/>
     <sheet name="UPS" sheetId="12" r:id="rId6"/>
     <sheet name="ContainerUPS" sheetId="13" r:id="rId7"/>
+    <sheet name="ERVAndARS" sheetId="14" r:id="rId8"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId8"/>
     <externalReference r:id="rId9"/>
+    <externalReference r:id="rId10"/>
   </externalReferences>
   <definedNames>
     <definedName name="CONF_UPS_Redundancy">[1]CONFIGURATOR!$D$28</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <oleSize ref="A1:Q10"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +33,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -44,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="234">
   <si>
     <t>TYPE</t>
   </si>
@@ -729,6 +728,24 @@
   </si>
   <si>
     <t>NON ISO45'</t>
+  </si>
+  <si>
+    <t>ERV / ARS</t>
+  </si>
+  <si>
+    <t>ARS_ISO</t>
+  </si>
+  <si>
+    <t>ISO20'_ETO</t>
+  </si>
+  <si>
+    <t>ISO40'_ETO</t>
+  </si>
+  <si>
+    <t>ARS_NONISO</t>
+  </si>
+  <si>
+    <t>NON ISOD45</t>
   </si>
 </sst>
 </file>
@@ -1094,7 +1111,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1229,9 +1246,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1260,6 +1274,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2697,10 +2720,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="74" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="62"/>
+      <c r="B1" s="74"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -4091,7 +4114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C54C99C0-56AC-4268-A6D1-0A84E8101377}">
   <dimension ref="A1:AC73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -4361,34 +4384,34 @@
       <c r="O14" s="61">
         <v>0</v>
       </c>
-      <c r="P14" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="63">
-        <v>0</v>
-      </c>
-      <c r="R14" s="63">
-        <v>0</v>
-      </c>
-      <c r="S14" s="63">
+      <c r="P14" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="62">
+        <v>0</v>
+      </c>
+      <c r="R14" s="62">
+        <v>0</v>
+      </c>
+      <c r="S14" s="62">
         <v>4</v>
       </c>
-      <c r="T14" s="63">
+      <c r="T14" s="62">
         <v>4</v>
       </c>
-      <c r="U14" s="64">
-        <v>0</v>
-      </c>
-      <c r="V14" s="63">
-        <v>0</v>
-      </c>
-      <c r="W14" s="63">
-        <v>0</v>
-      </c>
-      <c r="X14" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="63">
+      <c r="U14" s="63">
+        <v>0</v>
+      </c>
+      <c r="V14" s="62">
+        <v>0</v>
+      </c>
+      <c r="W14" s="62">
+        <v>0</v>
+      </c>
+      <c r="X14" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="62">
         <v>0</v>
       </c>
     </row>
@@ -4439,34 +4462,34 @@
       <c r="O15" s="61">
         <v>0</v>
       </c>
-      <c r="P15" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="63">
-        <v>0</v>
-      </c>
-      <c r="R15" s="63">
-        <v>0</v>
-      </c>
-      <c r="S15" s="63">
+      <c r="P15" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="62">
+        <v>0</v>
+      </c>
+      <c r="R15" s="62">
+        <v>0</v>
+      </c>
+      <c r="S15" s="62">
         <v>4</v>
       </c>
-      <c r="T15" s="63">
+      <c r="T15" s="62">
         <v>4</v>
       </c>
-      <c r="U15" s="64">
-        <v>0</v>
-      </c>
-      <c r="V15" s="63">
-        <v>0</v>
-      </c>
-      <c r="W15" s="63">
-        <v>0</v>
-      </c>
-      <c r="X15" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y15" s="63">
+      <c r="U15" s="63">
+        <v>0</v>
+      </c>
+      <c r="V15" s="62">
+        <v>0</v>
+      </c>
+      <c r="W15" s="62">
+        <v>0</v>
+      </c>
+      <c r="X15" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="62">
         <v>0</v>
       </c>
     </row>
@@ -4526,34 +4549,34 @@
       <c r="O16" s="61">
         <v>0</v>
       </c>
-      <c r="P16" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="63">
-        <v>0</v>
-      </c>
-      <c r="R16" s="63">
-        <v>0</v>
-      </c>
-      <c r="S16" s="63">
+      <c r="P16" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="62">
+        <v>0</v>
+      </c>
+      <c r="R16" s="62">
+        <v>0</v>
+      </c>
+      <c r="S16" s="62">
         <v>4</v>
       </c>
-      <c r="T16" s="63">
+      <c r="T16" s="62">
         <v>4</v>
       </c>
-      <c r="U16" s="64">
-        <v>0</v>
-      </c>
-      <c r="V16" s="63">
-        <v>0</v>
-      </c>
-      <c r="W16" s="63">
-        <v>0</v>
-      </c>
-      <c r="X16" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="63">
+      <c r="U16" s="63">
+        <v>0</v>
+      </c>
+      <c r="V16" s="62">
+        <v>0</v>
+      </c>
+      <c r="W16" s="62">
+        <v>0</v>
+      </c>
+      <c r="X16" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="62">
         <v>0</v>
       </c>
     </row>
@@ -4613,34 +4636,34 @@
       <c r="O17" s="61">
         <v>0</v>
       </c>
-      <c r="P17" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="63">
-        <v>0</v>
-      </c>
-      <c r="R17" s="63">
-        <v>0</v>
-      </c>
-      <c r="S17" s="63">
+      <c r="P17" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="62">
+        <v>0</v>
+      </c>
+      <c r="R17" s="62">
+        <v>0</v>
+      </c>
+      <c r="S17" s="62">
         <v>4</v>
       </c>
-      <c r="T17" s="63">
+      <c r="T17" s="62">
         <v>4</v>
       </c>
-      <c r="U17" s="64">
-        <v>0</v>
-      </c>
-      <c r="V17" s="63">
-        <v>0</v>
-      </c>
-      <c r="W17" s="63">
-        <v>0</v>
-      </c>
-      <c r="X17" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y17" s="63">
+      <c r="U17" s="63">
+        <v>0</v>
+      </c>
+      <c r="V17" s="62">
+        <v>0</v>
+      </c>
+      <c r="W17" s="62">
+        <v>0</v>
+      </c>
+      <c r="X17" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="62">
         <v>0</v>
       </c>
     </row>
@@ -4700,34 +4723,34 @@
       <c r="O18" s="61">
         <v>0</v>
       </c>
-      <c r="P18" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="63">
-        <v>0</v>
-      </c>
-      <c r="R18" s="63">
-        <v>0</v>
-      </c>
-      <c r="S18" s="63">
+      <c r="P18" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="62">
+        <v>0</v>
+      </c>
+      <c r="R18" s="62">
+        <v>0</v>
+      </c>
+      <c r="S18" s="62">
         <v>4</v>
       </c>
-      <c r="T18" s="63">
+      <c r="T18" s="62">
         <v>4</v>
       </c>
-      <c r="U18" s="64">
-        <v>0</v>
-      </c>
-      <c r="V18" s="63">
-        <v>0</v>
-      </c>
-      <c r="W18" s="63">
-        <v>0</v>
-      </c>
-      <c r="X18" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y18" s="63">
+      <c r="U18" s="63">
+        <v>0</v>
+      </c>
+      <c r="V18" s="62">
+        <v>0</v>
+      </c>
+      <c r="W18" s="62">
+        <v>0</v>
+      </c>
+      <c r="X18" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="62">
         <v>0</v>
       </c>
     </row>
@@ -4787,34 +4810,34 @@
       <c r="O19" s="61">
         <v>0</v>
       </c>
-      <c r="P19" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="63">
-        <v>0</v>
-      </c>
-      <c r="R19" s="63">
-        <v>0</v>
-      </c>
-      <c r="S19" s="63">
+      <c r="P19" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="62">
+        <v>0</v>
+      </c>
+      <c r="R19" s="62">
+        <v>0</v>
+      </c>
+      <c r="S19" s="62">
         <v>4</v>
       </c>
-      <c r="T19" s="63">
+      <c r="T19" s="62">
         <v>4</v>
       </c>
-      <c r="U19" s="64">
-        <v>0</v>
-      </c>
-      <c r="V19" s="63">
-        <v>0</v>
-      </c>
-      <c r="W19" s="63">
-        <v>0</v>
-      </c>
-      <c r="X19" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y19" s="63">
+      <c r="U19" s="63">
+        <v>0</v>
+      </c>
+      <c r="V19" s="62">
+        <v>0</v>
+      </c>
+      <c r="W19" s="62">
+        <v>0</v>
+      </c>
+      <c r="X19" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="62">
         <v>0</v>
       </c>
     </row>
@@ -4874,34 +4897,34 @@
       <c r="O20" s="61">
         <v>0</v>
       </c>
-      <c r="P20" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="63">
-        <v>0</v>
-      </c>
-      <c r="R20" s="63">
-        <v>0</v>
-      </c>
-      <c r="S20" s="63">
+      <c r="P20" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="62">
+        <v>0</v>
+      </c>
+      <c r="R20" s="62">
+        <v>0</v>
+      </c>
+      <c r="S20" s="62">
         <v>4</v>
       </c>
-      <c r="T20" s="63">
+      <c r="T20" s="62">
         <v>4</v>
       </c>
-      <c r="U20" s="64">
-        <v>0</v>
-      </c>
-      <c r="V20" s="63">
-        <v>0</v>
-      </c>
-      <c r="W20" s="63">
-        <v>0</v>
-      </c>
-      <c r="X20" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y20" s="63">
+      <c r="U20" s="63">
+        <v>0</v>
+      </c>
+      <c r="V20" s="62">
+        <v>0</v>
+      </c>
+      <c r="W20" s="62">
+        <v>0</v>
+      </c>
+      <c r="X20" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="62">
         <v>0</v>
       </c>
     </row>
@@ -4961,34 +4984,34 @@
       <c r="O21" s="61">
         <v>0</v>
       </c>
-      <c r="P21" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="63">
-        <v>0</v>
-      </c>
-      <c r="R21" s="63">
-        <v>0</v>
-      </c>
-      <c r="S21" s="63">
+      <c r="P21" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="62">
+        <v>0</v>
+      </c>
+      <c r="R21" s="62">
+        <v>0</v>
+      </c>
+      <c r="S21" s="62">
         <v>4</v>
       </c>
-      <c r="T21" s="63">
+      <c r="T21" s="62">
         <v>4</v>
       </c>
-      <c r="U21" s="64">
-        <v>0</v>
-      </c>
-      <c r="V21" s="63">
-        <v>0</v>
-      </c>
-      <c r="W21" s="63">
-        <v>0</v>
-      </c>
-      <c r="X21" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y21" s="63">
+      <c r="U21" s="63">
+        <v>0</v>
+      </c>
+      <c r="V21" s="62">
+        <v>0</v>
+      </c>
+      <c r="W21" s="62">
+        <v>0</v>
+      </c>
+      <c r="X21" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="62">
         <v>0</v>
       </c>
     </row>
@@ -5048,34 +5071,34 @@
       <c r="O22" s="61">
         <v>0</v>
       </c>
-      <c r="P22" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="63">
-        <v>0</v>
-      </c>
-      <c r="R22" s="63">
-        <v>0</v>
-      </c>
-      <c r="S22" s="63">
+      <c r="P22" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="62">
+        <v>0</v>
+      </c>
+      <c r="R22" s="62">
+        <v>0</v>
+      </c>
+      <c r="S22" s="62">
         <v>4</v>
       </c>
-      <c r="T22" s="63">
+      <c r="T22" s="62">
         <v>4</v>
       </c>
-      <c r="U22" s="64">
-        <v>0</v>
-      </c>
-      <c r="V22" s="63">
-        <v>0</v>
-      </c>
-      <c r="W22" s="63">
-        <v>0</v>
-      </c>
-      <c r="X22" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y22" s="63">
+      <c r="U22" s="63">
+        <v>0</v>
+      </c>
+      <c r="V22" s="62">
+        <v>0</v>
+      </c>
+      <c r="W22" s="62">
+        <v>0</v>
+      </c>
+      <c r="X22" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="62">
         <v>0</v>
       </c>
     </row>
@@ -5135,34 +5158,34 @@
       <c r="O23" s="61">
         <v>0</v>
       </c>
-      <c r="P23" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="63">
-        <v>0</v>
-      </c>
-      <c r="R23" s="63">
-        <v>0</v>
-      </c>
-      <c r="S23" s="65">
+      <c r="P23" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="62">
+        <v>0</v>
+      </c>
+      <c r="R23" s="62">
+        <v>0</v>
+      </c>
+      <c r="S23" s="64">
         <v>4</v>
       </c>
-      <c r="T23" s="65">
+      <c r="T23" s="64">
         <v>4</v>
       </c>
-      <c r="U23" s="64">
-        <v>0</v>
-      </c>
-      <c r="V23" s="63">
-        <v>0</v>
-      </c>
-      <c r="W23" s="63">
-        <v>0</v>
-      </c>
-      <c r="X23" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y23" s="63">
+      <c r="U23" s="63">
+        <v>0</v>
+      </c>
+      <c r="V23" s="62">
+        <v>0</v>
+      </c>
+      <c r="W23" s="62">
+        <v>0</v>
+      </c>
+      <c r="X23" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="62">
         <v>0</v>
       </c>
     </row>
@@ -5213,34 +5236,34 @@
       <c r="O24" s="61">
         <v>0</v>
       </c>
-      <c r="P24" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="63">
-        <v>0</v>
-      </c>
-      <c r="R24" s="63">
-        <v>0</v>
-      </c>
-      <c r="S24" s="66">
+      <c r="P24" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="62">
+        <v>0</v>
+      </c>
+      <c r="R24" s="62">
+        <v>0</v>
+      </c>
+      <c r="S24" s="65">
         <v>8</v>
       </c>
-      <c r="T24" s="66">
+      <c r="T24" s="65">
         <v>7</v>
       </c>
-      <c r="U24" s="64">
-        <v>0</v>
-      </c>
-      <c r="V24" s="63">
-        <v>0</v>
-      </c>
-      <c r="W24" s="63">
-        <v>0</v>
-      </c>
-      <c r="X24" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y24" s="63">
+      <c r="U24" s="63">
+        <v>0</v>
+      </c>
+      <c r="V24" s="62">
+        <v>0</v>
+      </c>
+      <c r="W24" s="62">
+        <v>0</v>
+      </c>
+      <c r="X24" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="62">
         <v>0</v>
       </c>
     </row>
@@ -5291,34 +5314,34 @@
       <c r="O25" s="61">
         <v>0</v>
       </c>
-      <c r="P25" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="63">
-        <v>0</v>
-      </c>
-      <c r="R25" s="63">
-        <v>0</v>
-      </c>
-      <c r="S25" s="66">
+      <c r="P25" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="62">
+        <v>0</v>
+      </c>
+      <c r="R25" s="62">
+        <v>0</v>
+      </c>
+      <c r="S25" s="65">
         <v>8</v>
       </c>
-      <c r="T25" s="66">
+      <c r="T25" s="65">
         <v>7</v>
       </c>
-      <c r="U25" s="64">
-        <v>0</v>
-      </c>
-      <c r="V25" s="63">
-        <v>0</v>
-      </c>
-      <c r="W25" s="63">
-        <v>0</v>
-      </c>
-      <c r="X25" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y25" s="63">
+      <c r="U25" s="63">
+        <v>0</v>
+      </c>
+      <c r="V25" s="62">
+        <v>0</v>
+      </c>
+      <c r="W25" s="62">
+        <v>0</v>
+      </c>
+      <c r="X25" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y25" s="62">
         <v>0</v>
       </c>
     </row>
@@ -5369,34 +5392,34 @@
       <c r="O26" s="61">
         <v>0</v>
       </c>
-      <c r="P26" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="63">
-        <v>0</v>
-      </c>
-      <c r="R26" s="63">
-        <v>0</v>
-      </c>
-      <c r="S26" s="66">
+      <c r="P26" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="62">
+        <v>0</v>
+      </c>
+      <c r="R26" s="62">
+        <v>0</v>
+      </c>
+      <c r="S26" s="65">
         <v>8</v>
       </c>
-      <c r="T26" s="66">
+      <c r="T26" s="65">
         <v>7</v>
       </c>
-      <c r="U26" s="64">
-        <v>0</v>
-      </c>
-      <c r="V26" s="63">
-        <v>0</v>
-      </c>
-      <c r="W26" s="63">
-        <v>0</v>
-      </c>
-      <c r="X26" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y26" s="63">
+      <c r="U26" s="63">
+        <v>0</v>
+      </c>
+      <c r="V26" s="62">
+        <v>0</v>
+      </c>
+      <c r="W26" s="62">
+        <v>0</v>
+      </c>
+      <c r="X26" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="62">
         <v>0</v>
       </c>
     </row>
@@ -5447,34 +5470,34 @@
       <c r="O27" s="61">
         <v>0</v>
       </c>
-      <c r="P27" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q27" s="63">
-        <v>0</v>
-      </c>
-      <c r="R27" s="63">
-        <v>0</v>
-      </c>
-      <c r="S27" s="66">
+      <c r="P27" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="62">
+        <v>0</v>
+      </c>
+      <c r="R27" s="62">
+        <v>0</v>
+      </c>
+      <c r="S27" s="65">
         <v>8</v>
       </c>
-      <c r="T27" s="66">
+      <c r="T27" s="65">
         <v>7</v>
       </c>
-      <c r="U27" s="64">
-        <v>0</v>
-      </c>
-      <c r="V27" s="63">
-        <v>0</v>
-      </c>
-      <c r="W27" s="63">
-        <v>0</v>
-      </c>
-      <c r="X27" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y27" s="63">
+      <c r="U27" s="63">
+        <v>0</v>
+      </c>
+      <c r="V27" s="62">
+        <v>0</v>
+      </c>
+      <c r="W27" s="62">
+        <v>0</v>
+      </c>
+      <c r="X27" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y27" s="62">
         <v>0</v>
       </c>
     </row>
@@ -5525,34 +5548,34 @@
       <c r="O28" s="61">
         <v>0</v>
       </c>
-      <c r="P28" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="63">
-        <v>0</v>
-      </c>
-      <c r="R28" s="63">
-        <v>0</v>
-      </c>
-      <c r="S28" s="66">
+      <c r="P28" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="62">
+        <v>0</v>
+      </c>
+      <c r="R28" s="62">
+        <v>0</v>
+      </c>
+      <c r="S28" s="65">
         <v>8</v>
       </c>
-      <c r="T28" s="66">
+      <c r="T28" s="65">
         <v>7</v>
       </c>
-      <c r="U28" s="64">
-        <v>0</v>
-      </c>
-      <c r="V28" s="63">
-        <v>0</v>
-      </c>
-      <c r="W28" s="63">
-        <v>0</v>
-      </c>
-      <c r="X28" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y28" s="63">
+      <c r="U28" s="63">
+        <v>0</v>
+      </c>
+      <c r="V28" s="62">
+        <v>0</v>
+      </c>
+      <c r="W28" s="62">
+        <v>0</v>
+      </c>
+      <c r="X28" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y28" s="62">
         <v>0</v>
       </c>
     </row>
@@ -5603,34 +5626,34 @@
       <c r="O29" s="61">
         <v>0</v>
       </c>
-      <c r="P29" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="63">
-        <v>0</v>
-      </c>
-      <c r="R29" s="63">
-        <v>0</v>
-      </c>
-      <c r="S29" s="66">
+      <c r="P29" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="62">
+        <v>0</v>
+      </c>
+      <c r="R29" s="62">
+        <v>0</v>
+      </c>
+      <c r="S29" s="65">
         <v>8</v>
       </c>
-      <c r="T29" s="66">
+      <c r="T29" s="65">
         <v>7</v>
       </c>
-      <c r="U29" s="64">
-        <v>0</v>
-      </c>
-      <c r="V29" s="63">
-        <v>0</v>
-      </c>
-      <c r="W29" s="63">
-        <v>0</v>
-      </c>
-      <c r="X29" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y29" s="63">
+      <c r="U29" s="63">
+        <v>0</v>
+      </c>
+      <c r="V29" s="62">
+        <v>0</v>
+      </c>
+      <c r="W29" s="62">
+        <v>0</v>
+      </c>
+      <c r="X29" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="62">
         <v>0</v>
       </c>
     </row>
@@ -5681,34 +5704,34 @@
       <c r="O30" s="61">
         <v>0</v>
       </c>
-      <c r="P30" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="63">
-        <v>0</v>
-      </c>
-      <c r="R30" s="63">
-        <v>0</v>
-      </c>
-      <c r="S30" s="66">
+      <c r="P30" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="62">
+        <v>0</v>
+      </c>
+      <c r="R30" s="62">
+        <v>0</v>
+      </c>
+      <c r="S30" s="65">
         <v>8</v>
       </c>
-      <c r="T30" s="66">
+      <c r="T30" s="65">
         <v>7</v>
       </c>
-      <c r="U30" s="64">
-        <v>0</v>
-      </c>
-      <c r="V30" s="63">
-        <v>0</v>
-      </c>
-      <c r="W30" s="63">
-        <v>0</v>
-      </c>
-      <c r="X30" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y30" s="63">
+      <c r="U30" s="63">
+        <v>0</v>
+      </c>
+      <c r="V30" s="62">
+        <v>0</v>
+      </c>
+      <c r="W30" s="62">
+        <v>0</v>
+      </c>
+      <c r="X30" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y30" s="62">
         <v>0</v>
       </c>
     </row>
@@ -5759,34 +5782,34 @@
       <c r="O31" s="61">
         <v>0</v>
       </c>
-      <c r="P31" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q31" s="63">
-        <v>0</v>
-      </c>
-      <c r="R31" s="63">
-        <v>0</v>
-      </c>
-      <c r="S31" s="66">
+      <c r="P31" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="62">
+        <v>0</v>
+      </c>
+      <c r="R31" s="62">
+        <v>0</v>
+      </c>
+      <c r="S31" s="65">
         <v>8</v>
       </c>
-      <c r="T31" s="66">
+      <c r="T31" s="65">
         <v>7</v>
       </c>
-      <c r="U31" s="64">
-        <v>0</v>
-      </c>
-      <c r="V31" s="63">
-        <v>0</v>
-      </c>
-      <c r="W31" s="63">
-        <v>0</v>
-      </c>
-      <c r="X31" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y31" s="63">
+      <c r="U31" s="63">
+        <v>0</v>
+      </c>
+      <c r="V31" s="62">
+        <v>0</v>
+      </c>
+      <c r="W31" s="62">
+        <v>0</v>
+      </c>
+      <c r="X31" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y31" s="62">
         <v>0</v>
       </c>
     </row>
@@ -5837,34 +5860,34 @@
       <c r="O32" s="61">
         <v>0</v>
       </c>
-      <c r="P32" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q32" s="63">
-        <v>0</v>
-      </c>
-      <c r="R32" s="63">
-        <v>0</v>
-      </c>
-      <c r="S32" s="66">
+      <c r="P32" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="62">
+        <v>0</v>
+      </c>
+      <c r="R32" s="62">
+        <v>0</v>
+      </c>
+      <c r="S32" s="65">
         <v>8</v>
       </c>
-      <c r="T32" s="66">
+      <c r="T32" s="65">
         <v>7</v>
       </c>
-      <c r="U32" s="64">
-        <v>0</v>
-      </c>
-      <c r="V32" s="63">
-        <v>0</v>
-      </c>
-      <c r="W32" s="63">
-        <v>0</v>
-      </c>
-      <c r="X32" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y32" s="63">
+      <c r="U32" s="63">
+        <v>0</v>
+      </c>
+      <c r="V32" s="62">
+        <v>0</v>
+      </c>
+      <c r="W32" s="62">
+        <v>0</v>
+      </c>
+      <c r="X32" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y32" s="62">
         <v>0</v>
       </c>
     </row>
@@ -5915,34 +5938,34 @@
       <c r="O33" s="61">
         <v>0</v>
       </c>
-      <c r="P33" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q33" s="63">
-        <v>0</v>
-      </c>
-      <c r="R33" s="63">
-        <v>0</v>
-      </c>
-      <c r="S33" s="65">
+      <c r="P33" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="62">
+        <v>0</v>
+      </c>
+      <c r="R33" s="62">
+        <v>0</v>
+      </c>
+      <c r="S33" s="64">
         <v>8</v>
       </c>
-      <c r="T33" s="65">
+      <c r="T33" s="64">
         <v>7</v>
       </c>
-      <c r="U33" s="64">
-        <v>0</v>
-      </c>
-      <c r="V33" s="63">
-        <v>0</v>
-      </c>
-      <c r="W33" s="63">
-        <v>0</v>
-      </c>
-      <c r="X33" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y33" s="63">
+      <c r="U33" s="63">
+        <v>0</v>
+      </c>
+      <c r="V33" s="62">
+        <v>0</v>
+      </c>
+      <c r="W33" s="62">
+        <v>0</v>
+      </c>
+      <c r="X33" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y33" s="62">
         <v>0</v>
       </c>
     </row>
@@ -6002,34 +6025,34 @@
       <c r="O34" s="61">
         <v>0</v>
       </c>
-      <c r="P34" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q34" s="63">
-        <v>0</v>
-      </c>
-      <c r="R34" s="63">
-        <v>0</v>
-      </c>
-      <c r="S34" s="66">
+      <c r="P34" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="62">
+        <v>0</v>
+      </c>
+      <c r="R34" s="62">
+        <v>0</v>
+      </c>
+      <c r="S34" s="65">
         <v>5</v>
       </c>
-      <c r="T34" s="66">
+      <c r="T34" s="65">
         <v>4</v>
       </c>
-      <c r="U34" s="64">
-        <v>0</v>
-      </c>
-      <c r="V34" s="63">
-        <v>0</v>
-      </c>
-      <c r="W34" s="63">
-        <v>0</v>
-      </c>
-      <c r="X34" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y34" s="63">
+      <c r="U34" s="63">
+        <v>0</v>
+      </c>
+      <c r="V34" s="62">
+        <v>0</v>
+      </c>
+      <c r="W34" s="62">
+        <v>0</v>
+      </c>
+      <c r="X34" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y34" s="62">
         <v>0</v>
       </c>
     </row>
@@ -6089,34 +6112,34 @@
       <c r="O35" s="61">
         <v>0</v>
       </c>
-      <c r="P35" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q35" s="63">
-        <v>0</v>
-      </c>
-      <c r="R35" s="63">
-        <v>0</v>
-      </c>
-      <c r="S35" s="66">
+      <c r="P35" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="62">
+        <v>0</v>
+      </c>
+      <c r="R35" s="62">
+        <v>0</v>
+      </c>
+      <c r="S35" s="65">
         <v>5</v>
       </c>
-      <c r="T35" s="66">
+      <c r="T35" s="65">
         <v>4</v>
       </c>
-      <c r="U35" s="64">
-        <v>0</v>
-      </c>
-      <c r="V35" s="63">
-        <v>0</v>
-      </c>
-      <c r="W35" s="63">
-        <v>0</v>
-      </c>
-      <c r="X35" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y35" s="63">
+      <c r="U35" s="63">
+        <v>0</v>
+      </c>
+      <c r="V35" s="62">
+        <v>0</v>
+      </c>
+      <c r="W35" s="62">
+        <v>0</v>
+      </c>
+      <c r="X35" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y35" s="62">
         <v>0</v>
       </c>
     </row>
@@ -6176,34 +6199,34 @@
       <c r="O36" s="61">
         <v>0</v>
       </c>
-      <c r="P36" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q36" s="63">
-        <v>0</v>
-      </c>
-      <c r="R36" s="63">
-        <v>0</v>
-      </c>
-      <c r="S36" s="66">
+      <c r="P36" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="62">
+        <v>0</v>
+      </c>
+      <c r="R36" s="62">
+        <v>0</v>
+      </c>
+      <c r="S36" s="65">
         <v>5</v>
       </c>
-      <c r="T36" s="66">
+      <c r="T36" s="65">
         <v>4</v>
       </c>
-      <c r="U36" s="64">
-        <v>0</v>
-      </c>
-      <c r="V36" s="63">
-        <v>0</v>
-      </c>
-      <c r="W36" s="63">
-        <v>0</v>
-      </c>
-      <c r="X36" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y36" s="63">
+      <c r="U36" s="63">
+        <v>0</v>
+      </c>
+      <c r="V36" s="62">
+        <v>0</v>
+      </c>
+      <c r="W36" s="62">
+        <v>0</v>
+      </c>
+      <c r="X36" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y36" s="62">
         <v>0</v>
       </c>
     </row>
@@ -6263,34 +6286,34 @@
       <c r="O37" s="61">
         <v>0</v>
       </c>
-      <c r="P37" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q37" s="63">
-        <v>0</v>
-      </c>
-      <c r="R37" s="63">
-        <v>0</v>
-      </c>
-      <c r="S37" s="66">
+      <c r="P37" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="62">
+        <v>0</v>
+      </c>
+      <c r="R37" s="62">
+        <v>0</v>
+      </c>
+      <c r="S37" s="65">
         <v>5</v>
       </c>
-      <c r="T37" s="66">
+      <c r="T37" s="65">
         <v>4</v>
       </c>
-      <c r="U37" s="64">
-        <v>0</v>
-      </c>
-      <c r="V37" s="63">
-        <v>0</v>
-      </c>
-      <c r="W37" s="63">
-        <v>0</v>
-      </c>
-      <c r="X37" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y37" s="63">
+      <c r="U37" s="63">
+        <v>0</v>
+      </c>
+      <c r="V37" s="62">
+        <v>0</v>
+      </c>
+      <c r="W37" s="62">
+        <v>0</v>
+      </c>
+      <c r="X37" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y37" s="62">
         <v>0</v>
       </c>
     </row>
@@ -6350,34 +6373,34 @@
       <c r="O38" s="61">
         <v>0</v>
       </c>
-      <c r="P38" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q38" s="63">
-        <v>0</v>
-      </c>
-      <c r="R38" s="63">
-        <v>0</v>
-      </c>
-      <c r="S38" s="66">
+      <c r="P38" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="62">
+        <v>0</v>
+      </c>
+      <c r="R38" s="62">
+        <v>0</v>
+      </c>
+      <c r="S38" s="65">
         <v>5</v>
       </c>
-      <c r="T38" s="66">
+      <c r="T38" s="65">
         <v>4</v>
       </c>
-      <c r="U38" s="64">
-        <v>0</v>
-      </c>
-      <c r="V38" s="63">
-        <v>0</v>
-      </c>
-      <c r="W38" s="63">
-        <v>0</v>
-      </c>
-      <c r="X38" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y38" s="63">
+      <c r="U38" s="63">
+        <v>0</v>
+      </c>
+      <c r="V38" s="62">
+        <v>0</v>
+      </c>
+      <c r="W38" s="62">
+        <v>0</v>
+      </c>
+      <c r="X38" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y38" s="62">
         <v>0</v>
       </c>
     </row>
@@ -6437,34 +6460,34 @@
       <c r="O39" s="61">
         <v>0</v>
       </c>
-      <c r="P39" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q39" s="63">
-        <v>0</v>
-      </c>
-      <c r="R39" s="63">
-        <v>0</v>
-      </c>
-      <c r="S39" s="66">
+      <c r="P39" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="62">
+        <v>0</v>
+      </c>
+      <c r="R39" s="62">
+        <v>0</v>
+      </c>
+      <c r="S39" s="65">
         <v>5</v>
       </c>
-      <c r="T39" s="66">
+      <c r="T39" s="65">
         <v>4</v>
       </c>
-      <c r="U39" s="64">
-        <v>0</v>
-      </c>
-      <c r="V39" s="63">
-        <v>0</v>
-      </c>
-      <c r="W39" s="63">
-        <v>0</v>
-      </c>
-      <c r="X39" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y39" s="63">
+      <c r="U39" s="63">
+        <v>0</v>
+      </c>
+      <c r="V39" s="62">
+        <v>0</v>
+      </c>
+      <c r="W39" s="62">
+        <v>0</v>
+      </c>
+      <c r="X39" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y39" s="62">
         <v>0</v>
       </c>
     </row>
@@ -6524,34 +6547,34 @@
       <c r="O40" s="61">
         <v>0</v>
       </c>
-      <c r="P40" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q40" s="63">
-        <v>0</v>
-      </c>
-      <c r="R40" s="63">
-        <v>0</v>
-      </c>
-      <c r="S40" s="66">
+      <c r="P40" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="62">
+        <v>0</v>
+      </c>
+      <c r="R40" s="62">
+        <v>0</v>
+      </c>
+      <c r="S40" s="65">
         <v>5</v>
       </c>
-      <c r="T40" s="66">
+      <c r="T40" s="65">
         <v>4</v>
       </c>
-      <c r="U40" s="64">
-        <v>0</v>
-      </c>
-      <c r="V40" s="63">
-        <v>0</v>
-      </c>
-      <c r="W40" s="63">
-        <v>0</v>
-      </c>
-      <c r="X40" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y40" s="63">
+      <c r="U40" s="63">
+        <v>0</v>
+      </c>
+      <c r="V40" s="62">
+        <v>0</v>
+      </c>
+      <c r="W40" s="62">
+        <v>0</v>
+      </c>
+      <c r="X40" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y40" s="62">
         <v>0</v>
       </c>
     </row>
@@ -6611,34 +6634,34 @@
       <c r="O41" s="61">
         <v>0</v>
       </c>
-      <c r="P41" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q41" s="63">
-        <v>0</v>
-      </c>
-      <c r="R41" s="63">
-        <v>0</v>
-      </c>
-      <c r="S41" s="66">
+      <c r="P41" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="62">
+        <v>0</v>
+      </c>
+      <c r="R41" s="62">
+        <v>0</v>
+      </c>
+      <c r="S41" s="65">
         <v>5</v>
       </c>
-      <c r="T41" s="66">
+      <c r="T41" s="65">
         <v>4</v>
       </c>
-      <c r="U41" s="64">
-        <v>0</v>
-      </c>
-      <c r="V41" s="63">
-        <v>0</v>
-      </c>
-      <c r="W41" s="63">
-        <v>0</v>
-      </c>
-      <c r="X41" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y41" s="63">
+      <c r="U41" s="63">
+        <v>0</v>
+      </c>
+      <c r="V41" s="62">
+        <v>0</v>
+      </c>
+      <c r="W41" s="62">
+        <v>0</v>
+      </c>
+      <c r="X41" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y41" s="62">
         <v>0</v>
       </c>
     </row>
@@ -6698,34 +6721,34 @@
       <c r="O42" s="61">
         <v>0</v>
       </c>
-      <c r="P42" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q42" s="63">
-        <v>0</v>
-      </c>
-      <c r="R42" s="63">
-        <v>0</v>
-      </c>
-      <c r="S42" s="66">
+      <c r="P42" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="62">
+        <v>0</v>
+      </c>
+      <c r="R42" s="62">
+        <v>0</v>
+      </c>
+      <c r="S42" s="65">
         <v>5</v>
       </c>
-      <c r="T42" s="66">
+      <c r="T42" s="65">
         <v>4</v>
       </c>
-      <c r="U42" s="64">
-        <v>0</v>
-      </c>
-      <c r="V42" s="63">
-        <v>0</v>
-      </c>
-      <c r="W42" s="63">
-        <v>0</v>
-      </c>
-      <c r="X42" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y42" s="63">
+      <c r="U42" s="63">
+        <v>0</v>
+      </c>
+      <c r="V42" s="62">
+        <v>0</v>
+      </c>
+      <c r="W42" s="62">
+        <v>0</v>
+      </c>
+      <c r="X42" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y42" s="62">
         <v>0</v>
       </c>
     </row>
@@ -6785,34 +6808,34 @@
       <c r="O43" s="61">
         <v>0</v>
       </c>
-      <c r="P43" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q43" s="63">
-        <v>0</v>
-      </c>
-      <c r="R43" s="63">
-        <v>0</v>
-      </c>
-      <c r="S43" s="65">
+      <c r="P43" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="62">
+        <v>0</v>
+      </c>
+      <c r="R43" s="62">
+        <v>0</v>
+      </c>
+      <c r="S43" s="64">
         <v>5</v>
       </c>
-      <c r="T43" s="65">
+      <c r="T43" s="64">
         <v>4</v>
       </c>
-      <c r="U43" s="64">
-        <v>0</v>
-      </c>
-      <c r="V43" s="63">
-        <v>0</v>
-      </c>
-      <c r="W43" s="63">
-        <v>0</v>
-      </c>
-      <c r="X43" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y43" s="63">
+      <c r="U43" s="63">
+        <v>0</v>
+      </c>
+      <c r="V43" s="62">
+        <v>0</v>
+      </c>
+      <c r="W43" s="62">
+        <v>0</v>
+      </c>
+      <c r="X43" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y43" s="62">
         <v>0</v>
       </c>
     </row>
@@ -6863,34 +6886,34 @@
       <c r="O44" s="61">
         <v>0</v>
       </c>
-      <c r="P44" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q44" s="63">
-        <v>0</v>
-      </c>
-      <c r="R44" s="63">
-        <v>0</v>
-      </c>
-      <c r="S44" s="66">
+      <c r="P44" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="62">
+        <v>0</v>
+      </c>
+      <c r="R44" s="62">
+        <v>0</v>
+      </c>
+      <c r="S44" s="65">
         <v>9</v>
       </c>
-      <c r="T44" s="66">
+      <c r="T44" s="65">
         <v>8</v>
       </c>
-      <c r="U44" s="64">
-        <v>0</v>
-      </c>
-      <c r="V44" s="63">
-        <v>0</v>
-      </c>
-      <c r="W44" s="63">
-        <v>0</v>
-      </c>
-      <c r="X44" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y44" s="63">
+      <c r="U44" s="63">
+        <v>0</v>
+      </c>
+      <c r="V44" s="62">
+        <v>0</v>
+      </c>
+      <c r="W44" s="62">
+        <v>0</v>
+      </c>
+      <c r="X44" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y44" s="62">
         <v>0</v>
       </c>
     </row>
@@ -6941,34 +6964,34 @@
       <c r="O45" s="61">
         <v>0</v>
       </c>
-      <c r="P45" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q45" s="63">
-        <v>0</v>
-      </c>
-      <c r="R45" s="63">
-        <v>0</v>
-      </c>
-      <c r="S45" s="66">
+      <c r="P45" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="62">
+        <v>0</v>
+      </c>
+      <c r="R45" s="62">
+        <v>0</v>
+      </c>
+      <c r="S45" s="65">
         <v>9</v>
       </c>
-      <c r="T45" s="66">
+      <c r="T45" s="65">
         <v>8</v>
       </c>
-      <c r="U45" s="64">
-        <v>0</v>
-      </c>
-      <c r="V45" s="63">
-        <v>0</v>
-      </c>
-      <c r="W45" s="63">
-        <v>0</v>
-      </c>
-      <c r="X45" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y45" s="63">
+      <c r="U45" s="63">
+        <v>0</v>
+      </c>
+      <c r="V45" s="62">
+        <v>0</v>
+      </c>
+      <c r="W45" s="62">
+        <v>0</v>
+      </c>
+      <c r="X45" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y45" s="62">
         <v>0</v>
       </c>
     </row>
@@ -7019,34 +7042,34 @@
       <c r="O46" s="61">
         <v>0</v>
       </c>
-      <c r="P46" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q46" s="63">
-        <v>0</v>
-      </c>
-      <c r="R46" s="63">
-        <v>0</v>
-      </c>
-      <c r="S46" s="66">
+      <c r="P46" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q46" s="62">
+        <v>0</v>
+      </c>
+      <c r="R46" s="62">
+        <v>0</v>
+      </c>
+      <c r="S46" s="65">
         <v>9</v>
       </c>
-      <c r="T46" s="66">
+      <c r="T46" s="65">
         <v>8</v>
       </c>
-      <c r="U46" s="64">
-        <v>0</v>
-      </c>
-      <c r="V46" s="63">
-        <v>0</v>
-      </c>
-      <c r="W46" s="63">
-        <v>0</v>
-      </c>
-      <c r="X46" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y46" s="63">
+      <c r="U46" s="63">
+        <v>0</v>
+      </c>
+      <c r="V46" s="62">
+        <v>0</v>
+      </c>
+      <c r="W46" s="62">
+        <v>0</v>
+      </c>
+      <c r="X46" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y46" s="62">
         <v>0</v>
       </c>
     </row>
@@ -7097,34 +7120,34 @@
       <c r="O47" s="61">
         <v>0</v>
       </c>
-      <c r="P47" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q47" s="63">
-        <v>0</v>
-      </c>
-      <c r="R47" s="63">
-        <v>0</v>
-      </c>
-      <c r="S47" s="66">
+      <c r="P47" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="62">
+        <v>0</v>
+      </c>
+      <c r="R47" s="62">
+        <v>0</v>
+      </c>
+      <c r="S47" s="65">
         <v>9</v>
       </c>
-      <c r="T47" s="66">
+      <c r="T47" s="65">
         <v>8</v>
       </c>
-      <c r="U47" s="64">
-        <v>0</v>
-      </c>
-      <c r="V47" s="63">
-        <v>0</v>
-      </c>
-      <c r="W47" s="63">
-        <v>0</v>
-      </c>
-      <c r="X47" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y47" s="63">
+      <c r="U47" s="63">
+        <v>0</v>
+      </c>
+      <c r="V47" s="62">
+        <v>0</v>
+      </c>
+      <c r="W47" s="62">
+        <v>0</v>
+      </c>
+      <c r="X47" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y47" s="62">
         <v>0</v>
       </c>
     </row>
@@ -7175,34 +7198,34 @@
       <c r="O48" s="61">
         <v>0</v>
       </c>
-      <c r="P48" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q48" s="63">
-        <v>0</v>
-      </c>
-      <c r="R48" s="63">
-        <v>0</v>
-      </c>
-      <c r="S48" s="66">
+      <c r="P48" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q48" s="62">
+        <v>0</v>
+      </c>
+      <c r="R48" s="62">
+        <v>0</v>
+      </c>
+      <c r="S48" s="65">
         <v>9</v>
       </c>
-      <c r="T48" s="66">
+      <c r="T48" s="65">
         <v>8</v>
       </c>
-      <c r="U48" s="64">
-        <v>0</v>
-      </c>
-      <c r="V48" s="63">
-        <v>0</v>
-      </c>
-      <c r="W48" s="63">
-        <v>0</v>
-      </c>
-      <c r="X48" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y48" s="63">
+      <c r="U48" s="63">
+        <v>0</v>
+      </c>
+      <c r="V48" s="62">
+        <v>0</v>
+      </c>
+      <c r="W48" s="62">
+        <v>0</v>
+      </c>
+      <c r="X48" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y48" s="62">
         <v>0</v>
       </c>
     </row>
@@ -7253,34 +7276,34 @@
       <c r="O49" s="61">
         <v>0</v>
       </c>
-      <c r="P49" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q49" s="63">
-        <v>0</v>
-      </c>
-      <c r="R49" s="63">
-        <v>0</v>
-      </c>
-      <c r="S49" s="66">
+      <c r="P49" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q49" s="62">
+        <v>0</v>
+      </c>
+      <c r="R49" s="62">
+        <v>0</v>
+      </c>
+      <c r="S49" s="65">
         <v>9</v>
       </c>
-      <c r="T49" s="66">
+      <c r="T49" s="65">
         <v>8</v>
       </c>
-      <c r="U49" s="64">
-        <v>0</v>
-      </c>
-      <c r="V49" s="63">
-        <v>0</v>
-      </c>
-      <c r="W49" s="63">
-        <v>0</v>
-      </c>
-      <c r="X49" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y49" s="63">
+      <c r="U49" s="63">
+        <v>0</v>
+      </c>
+      <c r="V49" s="62">
+        <v>0</v>
+      </c>
+      <c r="W49" s="62">
+        <v>0</v>
+      </c>
+      <c r="X49" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y49" s="62">
         <v>0</v>
       </c>
     </row>
@@ -7331,34 +7354,34 @@
       <c r="O50" s="61">
         <v>0</v>
       </c>
-      <c r="P50" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q50" s="63">
-        <v>0</v>
-      </c>
-      <c r="R50" s="63">
-        <v>0</v>
-      </c>
-      <c r="S50" s="66">
+      <c r="P50" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q50" s="62">
+        <v>0</v>
+      </c>
+      <c r="R50" s="62">
+        <v>0</v>
+      </c>
+      <c r="S50" s="65">
         <v>9</v>
       </c>
-      <c r="T50" s="66">
+      <c r="T50" s="65">
         <v>8</v>
       </c>
-      <c r="U50" s="64">
-        <v>0</v>
-      </c>
-      <c r="V50" s="63">
-        <v>0</v>
-      </c>
-      <c r="W50" s="63">
-        <v>0</v>
-      </c>
-      <c r="X50" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y50" s="63">
+      <c r="U50" s="63">
+        <v>0</v>
+      </c>
+      <c r="V50" s="62">
+        <v>0</v>
+      </c>
+      <c r="W50" s="62">
+        <v>0</v>
+      </c>
+      <c r="X50" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y50" s="62">
         <v>0</v>
       </c>
     </row>
@@ -7409,34 +7432,34 @@
       <c r="O51" s="61">
         <v>0</v>
       </c>
-      <c r="P51" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q51" s="63">
-        <v>0</v>
-      </c>
-      <c r="R51" s="63">
-        <v>0</v>
-      </c>
-      <c r="S51" s="66">
+      <c r="P51" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q51" s="62">
+        <v>0</v>
+      </c>
+      <c r="R51" s="62">
+        <v>0</v>
+      </c>
+      <c r="S51" s="65">
         <v>9</v>
       </c>
-      <c r="T51" s="66">
+      <c r="T51" s="65">
         <v>8</v>
       </c>
-      <c r="U51" s="64">
-        <v>0</v>
-      </c>
-      <c r="V51" s="63">
-        <v>0</v>
-      </c>
-      <c r="W51" s="63">
-        <v>0</v>
-      </c>
-      <c r="X51" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y51" s="63">
+      <c r="U51" s="63">
+        <v>0</v>
+      </c>
+      <c r="V51" s="62">
+        <v>0</v>
+      </c>
+      <c r="W51" s="62">
+        <v>0</v>
+      </c>
+      <c r="X51" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y51" s="62">
         <v>0</v>
       </c>
     </row>
@@ -7487,34 +7510,34 @@
       <c r="O52" s="61">
         <v>0</v>
       </c>
-      <c r="P52" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q52" s="63">
-        <v>0</v>
-      </c>
-      <c r="R52" s="63">
-        <v>0</v>
-      </c>
-      <c r="S52" s="66">
+      <c r="P52" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q52" s="62">
+        <v>0</v>
+      </c>
+      <c r="R52" s="62">
+        <v>0</v>
+      </c>
+      <c r="S52" s="65">
         <v>9</v>
       </c>
-      <c r="T52" s="66">
+      <c r="T52" s="65">
         <v>8</v>
       </c>
-      <c r="U52" s="64">
-        <v>0</v>
-      </c>
-      <c r="V52" s="63">
-        <v>0</v>
-      </c>
-      <c r="W52" s="63">
-        <v>0</v>
-      </c>
-      <c r="X52" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y52" s="63">
+      <c r="U52" s="63">
+        <v>0</v>
+      </c>
+      <c r="V52" s="62">
+        <v>0</v>
+      </c>
+      <c r="W52" s="62">
+        <v>0</v>
+      </c>
+      <c r="X52" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y52" s="62">
         <v>0</v>
       </c>
     </row>
@@ -7565,34 +7588,34 @@
       <c r="O53" s="61">
         <v>0</v>
       </c>
-      <c r="P53" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q53" s="63">
-        <v>0</v>
-      </c>
-      <c r="R53" s="63">
-        <v>0</v>
-      </c>
-      <c r="S53" s="65">
+      <c r="P53" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="62">
+        <v>0</v>
+      </c>
+      <c r="R53" s="62">
+        <v>0</v>
+      </c>
+      <c r="S53" s="64">
         <v>9</v>
       </c>
-      <c r="T53" s="65">
+      <c r="T53" s="64">
         <v>8</v>
       </c>
-      <c r="U53" s="64">
-        <v>0</v>
-      </c>
-      <c r="V53" s="63">
-        <v>0</v>
-      </c>
-      <c r="W53" s="63">
-        <v>0</v>
-      </c>
-      <c r="X53" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y53" s="63">
+      <c r="U53" s="63">
+        <v>0</v>
+      </c>
+      <c r="V53" s="62">
+        <v>0</v>
+      </c>
+      <c r="W53" s="62">
+        <v>0</v>
+      </c>
+      <c r="X53" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y53" s="62">
         <v>0</v>
       </c>
     </row>
@@ -7643,46 +7666,46 @@
       <c r="O54" s="56">
         <v>6120</v>
       </c>
-      <c r="P54" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q54" s="63">
-        <v>0</v>
-      </c>
-      <c r="R54" s="63">
-        <v>0</v>
-      </c>
-      <c r="S54" s="63">
+      <c r="P54" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="62">
+        <v>0</v>
+      </c>
+      <c r="R54" s="62">
+        <v>0</v>
+      </c>
+      <c r="S54" s="62">
         <v>12</v>
       </c>
-      <c r="T54" s="66">
+      <c r="T54" s="65">
         <v>8</v>
       </c>
-      <c r="U54" s="64">
-        <v>0</v>
-      </c>
-      <c r="V54" s="63">
-        <v>0</v>
-      </c>
-      <c r="W54" s="63">
-        <v>0</v>
-      </c>
-      <c r="X54" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y54" s="63">
-        <v>0</v>
-      </c>
-      <c r="Z54" s="67">
+      <c r="U54" s="63">
+        <v>0</v>
+      </c>
+      <c r="V54" s="62">
+        <v>0</v>
+      </c>
+      <c r="W54" s="62">
+        <v>0</v>
+      </c>
+      <c r="X54" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y54" s="62">
+        <v>0</v>
+      </c>
+      <c r="Z54" s="66">
         <v>3082</v>
       </c>
-      <c r="AA54" s="67">
+      <c r="AA54" s="66">
         <v>3082</v>
       </c>
-      <c r="AB54" s="70">
-        <v>0</v>
-      </c>
-      <c r="AC54" s="70">
+      <c r="AB54" s="69">
+        <v>0</v>
+      </c>
+      <c r="AC54" s="69">
         <v>0</v>
       </c>
     </row>
@@ -7733,46 +7756,46 @@
       <c r="O55" s="59">
         <v>6120</v>
       </c>
-      <c r="P55" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q55" s="63">
-        <v>0</v>
-      </c>
-      <c r="R55" s="63">
-        <v>0</v>
-      </c>
-      <c r="S55" s="63">
+      <c r="P55" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q55" s="62">
+        <v>0</v>
+      </c>
+      <c r="R55" s="62">
+        <v>0</v>
+      </c>
+      <c r="S55" s="62">
         <v>12</v>
       </c>
-      <c r="T55" s="66">
+      <c r="T55" s="65">
         <v>6</v>
       </c>
-      <c r="U55" s="64">
-        <v>0</v>
-      </c>
-      <c r="V55" s="63">
-        <v>0</v>
-      </c>
-      <c r="W55" s="63">
-        <v>0</v>
-      </c>
-      <c r="X55" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y55" s="63">
-        <v>0</v>
-      </c>
-      <c r="Z55" s="67">
+      <c r="U55" s="63">
+        <v>0</v>
+      </c>
+      <c r="V55" s="62">
+        <v>0</v>
+      </c>
+      <c r="W55" s="62">
+        <v>0</v>
+      </c>
+      <c r="X55" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y55" s="62">
+        <v>0</v>
+      </c>
+      <c r="Z55" s="66">
         <v>3320</v>
       </c>
-      <c r="AA55" s="67">
+      <c r="AA55" s="66">
         <v>3320</v>
       </c>
-      <c r="AB55" s="70">
+      <c r="AB55" s="69">
         <v>1074</v>
       </c>
-      <c r="AC55" s="70">
+      <c r="AC55" s="69">
         <v>1106</v>
       </c>
     </row>
@@ -7823,46 +7846,46 @@
       <c r="O56" s="59">
         <v>6120</v>
       </c>
-      <c r="P56" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q56" s="63">
-        <v>0</v>
-      </c>
-      <c r="R56" s="63">
-        <v>0</v>
-      </c>
-      <c r="S56" s="63">
+      <c r="P56" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q56" s="62">
+        <v>0</v>
+      </c>
+      <c r="R56" s="62">
+        <v>0</v>
+      </c>
+      <c r="S56" s="62">
         <v>12</v>
       </c>
-      <c r="T56" s="66">
+      <c r="T56" s="65">
         <v>8</v>
       </c>
-      <c r="U56" s="64">
-        <v>0</v>
-      </c>
-      <c r="V56" s="63">
-        <v>0</v>
-      </c>
-      <c r="W56" s="63">
-        <v>0</v>
-      </c>
-      <c r="X56" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y56" s="63">
-        <v>0</v>
-      </c>
-      <c r="Z56" s="67">
+      <c r="U56" s="63">
+        <v>0</v>
+      </c>
+      <c r="V56" s="62">
+        <v>0</v>
+      </c>
+      <c r="W56" s="62">
+        <v>0</v>
+      </c>
+      <c r="X56" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y56" s="62">
+        <v>0</v>
+      </c>
+      <c r="Z56" s="66">
         <v>3082</v>
       </c>
-      <c r="AA56" s="67">
+      <c r="AA56" s="66">
         <v>3082</v>
       </c>
-      <c r="AB56" s="70">
-        <v>0</v>
-      </c>
-      <c r="AC56" s="70">
+      <c r="AB56" s="69">
+        <v>0</v>
+      </c>
+      <c r="AC56" s="69">
         <v>0</v>
       </c>
     </row>
@@ -7913,46 +7936,46 @@
       <c r="O57" s="59">
         <v>6120</v>
       </c>
-      <c r="P57" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q57" s="63">
-        <v>0</v>
-      </c>
-      <c r="R57" s="63">
-        <v>0</v>
-      </c>
-      <c r="S57" s="63">
+      <c r="P57" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q57" s="62">
+        <v>0</v>
+      </c>
+      <c r="R57" s="62">
+        <v>0</v>
+      </c>
+      <c r="S57" s="62">
         <v>12</v>
       </c>
-      <c r="T57" s="66">
+      <c r="T57" s="65">
         <v>8</v>
       </c>
-      <c r="U57" s="64">
-        <v>0</v>
-      </c>
-      <c r="V57" s="63">
-        <v>0</v>
-      </c>
-      <c r="W57" s="63">
-        <v>0</v>
-      </c>
-      <c r="X57" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y57" s="63">
-        <v>0</v>
-      </c>
-      <c r="Z57" s="67">
+      <c r="U57" s="63">
+        <v>0</v>
+      </c>
+      <c r="V57" s="62">
+        <v>0</v>
+      </c>
+      <c r="W57" s="62">
+        <v>0</v>
+      </c>
+      <c r="X57" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y57" s="62">
+        <v>0</v>
+      </c>
+      <c r="Z57" s="66">
         <v>2725</v>
       </c>
-      <c r="AA57" s="67">
+      <c r="AA57" s="66">
         <v>2725</v>
       </c>
-      <c r="AB57" s="70">
+      <c r="AB57" s="69">
         <v>1106</v>
       </c>
-      <c r="AC57" s="70">
+      <c r="AC57" s="69">
         <v>1106</v>
       </c>
     </row>
@@ -8003,46 +8026,46 @@
       <c r="O58" s="59">
         <v>6120</v>
       </c>
-      <c r="P58" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q58" s="63">
-        <v>0</v>
-      </c>
-      <c r="R58" s="63">
-        <v>0</v>
-      </c>
-      <c r="S58" s="63">
+      <c r="P58" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q58" s="62">
+        <v>0</v>
+      </c>
+      <c r="R58" s="62">
+        <v>0</v>
+      </c>
+      <c r="S58" s="62">
         <v>12</v>
       </c>
-      <c r="T58" s="66">
+      <c r="T58" s="65">
         <v>8</v>
       </c>
-      <c r="U58" s="64">
-        <v>0</v>
-      </c>
-      <c r="V58" s="63">
-        <v>0</v>
-      </c>
-      <c r="W58" s="63">
-        <v>0</v>
-      </c>
-      <c r="X58" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y58" s="63">
-        <v>0</v>
-      </c>
-      <c r="Z58" s="67">
+      <c r="U58" s="63">
+        <v>0</v>
+      </c>
+      <c r="V58" s="62">
+        <v>0</v>
+      </c>
+      <c r="W58" s="62">
+        <v>0</v>
+      </c>
+      <c r="X58" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y58" s="62">
+        <v>0</v>
+      </c>
+      <c r="Z58" s="66">
         <v>3082</v>
       </c>
-      <c r="AA58" s="67">
+      <c r="AA58" s="66">
         <v>3082</v>
       </c>
-      <c r="AB58" s="70">
-        <v>0</v>
-      </c>
-      <c r="AC58" s="70">
+      <c r="AB58" s="69">
+        <v>0</v>
+      </c>
+      <c r="AC58" s="69">
         <v>0</v>
       </c>
     </row>
@@ -8093,46 +8116,46 @@
       <c r="O59" s="59">
         <v>6120</v>
       </c>
-      <c r="P59" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q59" s="63">
-        <v>0</v>
-      </c>
-      <c r="R59" s="63">
-        <v>0</v>
-      </c>
-      <c r="S59" s="63">
+      <c r="P59" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q59" s="62">
+        <v>0</v>
+      </c>
+      <c r="R59" s="62">
+        <v>0</v>
+      </c>
+      <c r="S59" s="62">
         <v>12</v>
       </c>
-      <c r="T59" s="66">
+      <c r="T59" s="65">
         <v>8</v>
       </c>
-      <c r="U59" s="64">
-        <v>0</v>
-      </c>
-      <c r="V59" s="63">
-        <v>0</v>
-      </c>
-      <c r="W59" s="63">
-        <v>0</v>
-      </c>
-      <c r="X59" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y59" s="63">
-        <v>0</v>
-      </c>
-      <c r="Z59" s="67">
+      <c r="U59" s="63">
+        <v>0</v>
+      </c>
+      <c r="V59" s="62">
+        <v>0</v>
+      </c>
+      <c r="W59" s="62">
+        <v>0</v>
+      </c>
+      <c r="X59" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y59" s="62">
+        <v>0</v>
+      </c>
+      <c r="Z59" s="66">
         <v>2725</v>
       </c>
-      <c r="AA59" s="67">
+      <c r="AA59" s="66">
         <v>2725</v>
       </c>
-      <c r="AB59" s="70">
+      <c r="AB59" s="69">
         <v>1106</v>
       </c>
-      <c r="AC59" s="70">
+      <c r="AC59" s="69">
         <v>1106</v>
       </c>
     </row>
@@ -8183,46 +8206,46 @@
       <c r="O60" s="59">
         <v>6120</v>
       </c>
-      <c r="P60" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q60" s="63">
-        <v>0</v>
-      </c>
-      <c r="R60" s="63">
-        <v>0</v>
-      </c>
-      <c r="S60" s="63">
+      <c r="P60" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q60" s="62">
+        <v>0</v>
+      </c>
+      <c r="R60" s="62">
+        <v>0</v>
+      </c>
+      <c r="S60" s="62">
         <v>12</v>
       </c>
-      <c r="T60" s="66">
+      <c r="T60" s="65">
         <v>8</v>
       </c>
-      <c r="U60" s="64">
-        <v>0</v>
-      </c>
-      <c r="V60" s="63">
-        <v>0</v>
-      </c>
-      <c r="W60" s="63">
-        <v>0</v>
-      </c>
-      <c r="X60" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y60" s="63">
-        <v>0</v>
-      </c>
-      <c r="Z60" s="67">
+      <c r="U60" s="63">
+        <v>0</v>
+      </c>
+      <c r="V60" s="62">
+        <v>0</v>
+      </c>
+      <c r="W60" s="62">
+        <v>0</v>
+      </c>
+      <c r="X60" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y60" s="62">
+        <v>0</v>
+      </c>
+      <c r="Z60" s="66">
         <v>1036</v>
       </c>
-      <c r="AA60" s="67">
+      <c r="AA60" s="66">
         <v>1036</v>
       </c>
-      <c r="AB60" s="70">
-        <v>0</v>
-      </c>
-      <c r="AC60" s="70">
+      <c r="AB60" s="69">
+        <v>0</v>
+      </c>
+      <c r="AC60" s="69">
         <v>0</v>
       </c>
     </row>
@@ -8273,46 +8296,46 @@
       <c r="O61" s="59">
         <v>6120</v>
       </c>
-      <c r="P61" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q61" s="63">
-        <v>0</v>
-      </c>
-      <c r="R61" s="63">
-        <v>0</v>
-      </c>
-      <c r="S61" s="63">
+      <c r="P61" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q61" s="62">
+        <v>0</v>
+      </c>
+      <c r="R61" s="62">
+        <v>0</v>
+      </c>
+      <c r="S61" s="62">
         <v>12</v>
       </c>
-      <c r="T61" s="66">
+      <c r="T61" s="65">
         <v>8</v>
       </c>
-      <c r="U61" s="64">
-        <v>0</v>
-      </c>
-      <c r="V61" s="63">
-        <v>0</v>
-      </c>
-      <c r="W61" s="63">
-        <v>0</v>
-      </c>
-      <c r="X61" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y61" s="63">
-        <v>0</v>
-      </c>
-      <c r="Z61" s="67">
+      <c r="U61" s="63">
+        <v>0</v>
+      </c>
+      <c r="V61" s="62">
+        <v>0</v>
+      </c>
+      <c r="W61" s="62">
+        <v>0</v>
+      </c>
+      <c r="X61" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y61" s="62">
+        <v>0</v>
+      </c>
+      <c r="Z61" s="66">
         <v>2013</v>
       </c>
-      <c r="AA61" s="67">
+      <c r="AA61" s="66">
         <v>2013</v>
       </c>
-      <c r="AB61" s="70">
-        <v>0</v>
-      </c>
-      <c r="AC61" s="70">
+      <c r="AB61" s="69">
+        <v>0</v>
+      </c>
+      <c r="AC61" s="69">
         <v>0</v>
       </c>
     </row>
@@ -8363,46 +8386,46 @@
       <c r="O62" s="59">
         <v>6120</v>
       </c>
-      <c r="P62" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q62" s="63">
-        <v>0</v>
-      </c>
-      <c r="R62" s="63">
-        <v>0</v>
-      </c>
-      <c r="S62" s="63">
+      <c r="P62" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q62" s="62">
+        <v>0</v>
+      </c>
+      <c r="R62" s="62">
+        <v>0</v>
+      </c>
+      <c r="S62" s="62">
         <v>12</v>
       </c>
-      <c r="T62" s="66">
+      <c r="T62" s="65">
         <v>8</v>
       </c>
-      <c r="U62" s="64">
-        <v>0</v>
-      </c>
-      <c r="V62" s="63">
-        <v>0</v>
-      </c>
-      <c r="W62" s="63">
-        <v>0</v>
-      </c>
-      <c r="X62" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y62" s="63">
-        <v>0</v>
-      </c>
-      <c r="Z62" s="68">
+      <c r="U62" s="63">
+        <v>0</v>
+      </c>
+      <c r="V62" s="62">
+        <v>0</v>
+      </c>
+      <c r="W62" s="62">
+        <v>0</v>
+      </c>
+      <c r="X62" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y62" s="62">
+        <v>0</v>
+      </c>
+      <c r="Z62" s="67">
         <v>1036</v>
       </c>
-      <c r="AA62" s="68">
+      <c r="AA62" s="67">
         <v>1036</v>
       </c>
-      <c r="AB62" s="71">
-        <v>0</v>
-      </c>
-      <c r="AC62" s="71">
+      <c r="AB62" s="70">
+        <v>0</v>
+      </c>
+      <c r="AC62" s="70">
         <v>0</v>
       </c>
     </row>
@@ -8453,46 +8476,46 @@
       <c r="O63" s="53">
         <v>6120</v>
       </c>
-      <c r="P63" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q63" s="63">
-        <v>0</v>
-      </c>
-      <c r="R63" s="63">
-        <v>0</v>
-      </c>
-      <c r="S63" s="65">
+      <c r="P63" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q63" s="62">
+        <v>0</v>
+      </c>
+      <c r="R63" s="62">
+        <v>0</v>
+      </c>
+      <c r="S63" s="64">
         <v>12</v>
       </c>
-      <c r="T63" s="65">
+      <c r="T63" s="64">
         <v>8</v>
       </c>
-      <c r="U63" s="64">
-        <v>0</v>
-      </c>
-      <c r="V63" s="63">
-        <v>0</v>
-      </c>
-      <c r="W63" s="63">
-        <v>0</v>
-      </c>
-      <c r="X63" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y63" s="63">
-        <v>0</v>
-      </c>
-      <c r="Z63" s="69">
+      <c r="U63" s="63">
+        <v>0</v>
+      </c>
+      <c r="V63" s="62">
+        <v>0</v>
+      </c>
+      <c r="W63" s="62">
+        <v>0</v>
+      </c>
+      <c r="X63" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y63" s="62">
+        <v>0</v>
+      </c>
+      <c r="Z63" s="68">
         <v>2013</v>
       </c>
-      <c r="AA63" s="69">
+      <c r="AA63" s="68">
         <v>2013</v>
       </c>
-      <c r="AB63" s="72">
-        <v>0</v>
-      </c>
-      <c r="AC63" s="72">
+      <c r="AB63" s="71">
+        <v>0</v>
+      </c>
+      <c r="AC63" s="71">
         <v>0</v>
       </c>
     </row>
@@ -8543,46 +8566,46 @@
       <c r="O64" s="56">
         <v>12260</v>
       </c>
-      <c r="P64" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q64" s="63">
-        <v>0</v>
-      </c>
-      <c r="R64" s="63">
-        <v>0</v>
-      </c>
-      <c r="S64" s="66">
+      <c r="P64" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q64" s="62">
+        <v>0</v>
+      </c>
+      <c r="R64" s="62">
+        <v>0</v>
+      </c>
+      <c r="S64" s="65">
         <v>20</v>
       </c>
-      <c r="T64" s="66">
+      <c r="T64" s="65">
         <v>14</v>
       </c>
-      <c r="U64" s="64">
-        <v>0</v>
-      </c>
-      <c r="V64" s="63">
-        <v>0</v>
-      </c>
-      <c r="W64" s="63">
-        <v>0</v>
-      </c>
-      <c r="X64" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y64" s="63">
-        <v>0</v>
-      </c>
-      <c r="Z64" s="67">
+      <c r="U64" s="63">
+        <v>0</v>
+      </c>
+      <c r="V64" s="62">
+        <v>0</v>
+      </c>
+      <c r="W64" s="62">
+        <v>0</v>
+      </c>
+      <c r="X64" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y64" s="62">
+        <v>0</v>
+      </c>
+      <c r="Z64" s="66">
         <v>3082</v>
       </c>
-      <c r="AA64" s="67">
+      <c r="AA64" s="66">
         <v>3082</v>
       </c>
-      <c r="AB64" s="70">
-        <v>0</v>
-      </c>
-      <c r="AC64" s="70">
+      <c r="AB64" s="69">
+        <v>0</v>
+      </c>
+      <c r="AC64" s="69">
         <v>0</v>
       </c>
     </row>
@@ -8633,46 +8656,46 @@
       <c r="O65" s="59">
         <v>12260</v>
       </c>
-      <c r="P65" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q65" s="63">
-        <v>0</v>
-      </c>
-      <c r="R65" s="63">
-        <v>0</v>
-      </c>
-      <c r="S65" s="66">
+      <c r="P65" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q65" s="62">
+        <v>0</v>
+      </c>
+      <c r="R65" s="62">
+        <v>0</v>
+      </c>
+      <c r="S65" s="65">
         <v>20</v>
       </c>
-      <c r="T65" s="66">
+      <c r="T65" s="65">
         <v>12</v>
       </c>
-      <c r="U65" s="64">
-        <v>0</v>
-      </c>
-      <c r="V65" s="63">
-        <v>0</v>
-      </c>
-      <c r="W65" s="63">
-        <v>0</v>
-      </c>
-      <c r="X65" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y65" s="63">
-        <v>0</v>
-      </c>
-      <c r="Z65" s="67">
+      <c r="U65" s="63">
+        <v>0</v>
+      </c>
+      <c r="V65" s="62">
+        <v>0</v>
+      </c>
+      <c r="W65" s="62">
+        <v>0</v>
+      </c>
+      <c r="X65" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y65" s="62">
+        <v>0</v>
+      </c>
+      <c r="Z65" s="66">
         <v>3320</v>
       </c>
-      <c r="AA65" s="67">
+      <c r="AA65" s="66">
         <v>3320</v>
       </c>
-      <c r="AB65" s="70">
+      <c r="AB65" s="69">
         <v>1106</v>
       </c>
-      <c r="AC65" s="70">
+      <c r="AC65" s="69">
         <v>1106</v>
       </c>
     </row>
@@ -8723,46 +8746,46 @@
       <c r="O66" s="59">
         <v>12260</v>
       </c>
-      <c r="P66" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q66" s="63">
-        <v>0</v>
-      </c>
-      <c r="R66" s="63">
-        <v>0</v>
-      </c>
-      <c r="S66" s="66">
+      <c r="P66" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q66" s="62">
+        <v>0</v>
+      </c>
+      <c r="R66" s="62">
+        <v>0</v>
+      </c>
+      <c r="S66" s="65">
         <v>20</v>
       </c>
-      <c r="T66" s="66">
+      <c r="T66" s="65">
         <v>14</v>
       </c>
-      <c r="U66" s="64">
-        <v>0</v>
-      </c>
-      <c r="V66" s="63">
-        <v>0</v>
-      </c>
-      <c r="W66" s="63">
-        <v>0</v>
-      </c>
-      <c r="X66" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y66" s="63">
-        <v>0</v>
-      </c>
-      <c r="Z66" s="67">
+      <c r="U66" s="63">
+        <v>0</v>
+      </c>
+      <c r="V66" s="62">
+        <v>0</v>
+      </c>
+      <c r="W66" s="62">
+        <v>0</v>
+      </c>
+      <c r="X66" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y66" s="62">
+        <v>0</v>
+      </c>
+      <c r="Z66" s="66">
         <v>3082</v>
       </c>
-      <c r="AA66" s="67">
+      <c r="AA66" s="66">
         <v>3082</v>
       </c>
-      <c r="AB66" s="70">
-        <v>0</v>
-      </c>
-      <c r="AC66" s="70">
+      <c r="AB66" s="69">
+        <v>0</v>
+      </c>
+      <c r="AC66" s="69">
         <v>0</v>
       </c>
     </row>
@@ -8813,46 +8836,46 @@
       <c r="O67" s="59">
         <v>12260</v>
       </c>
-      <c r="P67" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q67" s="63">
-        <v>0</v>
-      </c>
-      <c r="R67" s="63">
-        <v>0</v>
-      </c>
-      <c r="S67" s="66">
+      <c r="P67" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q67" s="62">
+        <v>0</v>
+      </c>
+      <c r="R67" s="62">
+        <v>0</v>
+      </c>
+      <c r="S67" s="65">
         <v>20</v>
       </c>
-      <c r="T67" s="66">
+      <c r="T67" s="65">
         <v>12</v>
       </c>
-      <c r="U67" s="64">
-        <v>0</v>
-      </c>
-      <c r="V67" s="63">
-        <v>0</v>
-      </c>
-      <c r="W67" s="63">
-        <v>0</v>
-      </c>
-      <c r="X67" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y67" s="63">
-        <v>0</v>
-      </c>
-      <c r="Z67" s="67">
+      <c r="U67" s="63">
+        <v>0</v>
+      </c>
+      <c r="V67" s="62">
+        <v>0</v>
+      </c>
+      <c r="W67" s="62">
+        <v>0</v>
+      </c>
+      <c r="X67" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y67" s="62">
+        <v>0</v>
+      </c>
+      <c r="Z67" s="66">
         <v>2725</v>
       </c>
-      <c r="AA67" s="67">
+      <c r="AA67" s="66">
         <v>2725</v>
       </c>
-      <c r="AB67" s="70">
+      <c r="AB67" s="69">
         <v>1106</v>
       </c>
-      <c r="AC67" s="70">
+      <c r="AC67" s="69">
         <v>1106</v>
       </c>
     </row>
@@ -8903,46 +8926,46 @@
       <c r="O68" s="59">
         <v>12260</v>
       </c>
-      <c r="P68" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q68" s="63">
-        <v>0</v>
-      </c>
-      <c r="R68" s="63">
-        <v>0</v>
-      </c>
-      <c r="S68" s="66">
+      <c r="P68" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q68" s="62">
+        <v>0</v>
+      </c>
+      <c r="R68" s="62">
+        <v>0</v>
+      </c>
+      <c r="S68" s="65">
         <v>20</v>
       </c>
-      <c r="T68" s="66">
+      <c r="T68" s="65">
         <v>14</v>
       </c>
-      <c r="U68" s="64">
-        <v>0</v>
-      </c>
-      <c r="V68" s="63">
-        <v>0</v>
-      </c>
-      <c r="W68" s="63">
-        <v>0</v>
-      </c>
-      <c r="X68" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y68" s="63">
-        <v>0</v>
-      </c>
-      <c r="Z68" s="67">
+      <c r="U68" s="63">
+        <v>0</v>
+      </c>
+      <c r="V68" s="62">
+        <v>0</v>
+      </c>
+      <c r="W68" s="62">
+        <v>0</v>
+      </c>
+      <c r="X68" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y68" s="62">
+        <v>0</v>
+      </c>
+      <c r="Z68" s="66">
         <v>3082</v>
       </c>
-      <c r="AA68" s="67">
+      <c r="AA68" s="66">
         <v>3082</v>
       </c>
-      <c r="AB68" s="70">
-        <v>0</v>
-      </c>
-      <c r="AC68" s="70">
+      <c r="AB68" s="69">
+        <v>0</v>
+      </c>
+      <c r="AC68" s="69">
         <v>0</v>
       </c>
     </row>
@@ -8993,46 +9016,46 @@
       <c r="O69" s="59">
         <v>12260</v>
       </c>
-      <c r="P69" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q69" s="63">
-        <v>0</v>
-      </c>
-      <c r="R69" s="63">
-        <v>0</v>
-      </c>
-      <c r="S69" s="66">
+      <c r="P69" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q69" s="62">
+        <v>0</v>
+      </c>
+      <c r="R69" s="62">
+        <v>0</v>
+      </c>
+      <c r="S69" s="65">
         <v>20</v>
       </c>
-      <c r="T69" s="66">
+      <c r="T69" s="65">
         <v>12</v>
       </c>
-      <c r="U69" s="64">
-        <v>0</v>
-      </c>
-      <c r="V69" s="63">
-        <v>0</v>
-      </c>
-      <c r="W69" s="63">
-        <v>0</v>
-      </c>
-      <c r="X69" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y69" s="63">
-        <v>0</v>
-      </c>
-      <c r="Z69" s="67">
+      <c r="U69" s="63">
+        <v>0</v>
+      </c>
+      <c r="V69" s="62">
+        <v>0</v>
+      </c>
+      <c r="W69" s="62">
+        <v>0</v>
+      </c>
+      <c r="X69" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y69" s="62">
+        <v>0</v>
+      </c>
+      <c r="Z69" s="66">
         <v>2725</v>
       </c>
-      <c r="AA69" s="67">
+      <c r="AA69" s="66">
         <v>2725</v>
       </c>
-      <c r="AB69" s="70">
+      <c r="AB69" s="69">
         <v>1106</v>
       </c>
-      <c r="AC69" s="70">
+      <c r="AC69" s="69">
         <v>1106</v>
       </c>
     </row>
@@ -9083,46 +9106,46 @@
       <c r="O70" s="59">
         <v>12260</v>
       </c>
-      <c r="P70" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q70" s="63">
-        <v>0</v>
-      </c>
-      <c r="R70" s="63">
-        <v>0</v>
-      </c>
-      <c r="S70" s="66">
+      <c r="P70" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q70" s="62">
+        <v>0</v>
+      </c>
+      <c r="R70" s="62">
+        <v>0</v>
+      </c>
+      <c r="S70" s="65">
         <v>20</v>
       </c>
-      <c r="T70" s="66">
+      <c r="T70" s="65">
         <v>14</v>
       </c>
-      <c r="U70" s="64">
-        <v>0</v>
-      </c>
-      <c r="V70" s="63">
-        <v>0</v>
-      </c>
-      <c r="W70" s="63">
-        <v>0</v>
-      </c>
-      <c r="X70" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y70" s="63">
-        <v>0</v>
-      </c>
-      <c r="Z70" s="67">
+      <c r="U70" s="63">
+        <v>0</v>
+      </c>
+      <c r="V70" s="62">
+        <v>0</v>
+      </c>
+      <c r="W70" s="62">
+        <v>0</v>
+      </c>
+      <c r="X70" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y70" s="62">
+        <v>0</v>
+      </c>
+      <c r="Z70" s="66">
         <v>1036</v>
       </c>
-      <c r="AA70" s="67">
+      <c r="AA70" s="66">
         <v>1036</v>
       </c>
-      <c r="AB70" s="70">
-        <v>0</v>
-      </c>
-      <c r="AC70" s="70">
+      <c r="AB70" s="69">
+        <v>0</v>
+      </c>
+      <c r="AC70" s="69">
         <v>0</v>
       </c>
     </row>
@@ -9173,46 +9196,46 @@
       <c r="O71" s="59">
         <v>12260</v>
       </c>
-      <c r="P71" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q71" s="63">
-        <v>0</v>
-      </c>
-      <c r="R71" s="63">
-        <v>0</v>
-      </c>
-      <c r="S71" s="66">
+      <c r="P71" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q71" s="62">
+        <v>0</v>
+      </c>
+      <c r="R71" s="62">
+        <v>0</v>
+      </c>
+      <c r="S71" s="65">
         <v>20</v>
       </c>
-      <c r="T71" s="66">
+      <c r="T71" s="65">
         <v>12</v>
       </c>
-      <c r="U71" s="64">
-        <v>0</v>
-      </c>
-      <c r="V71" s="63">
-        <v>0</v>
-      </c>
-      <c r="W71" s="63">
-        <v>0</v>
-      </c>
-      <c r="X71" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y71" s="63">
-        <v>0</v>
-      </c>
-      <c r="Z71" s="67">
+      <c r="U71" s="63">
+        <v>0</v>
+      </c>
+      <c r="V71" s="62">
+        <v>0</v>
+      </c>
+      <c r="W71" s="62">
+        <v>0</v>
+      </c>
+      <c r="X71" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y71" s="62">
+        <v>0</v>
+      </c>
+      <c r="Z71" s="66">
         <v>2013</v>
       </c>
-      <c r="AA71" s="67">
+      <c r="AA71" s="66">
         <v>2013</v>
       </c>
-      <c r="AB71" s="70">
-        <v>0</v>
-      </c>
-      <c r="AC71" s="70">
+      <c r="AB71" s="69">
+        <v>0</v>
+      </c>
+      <c r="AC71" s="69">
         <v>0</v>
       </c>
     </row>
@@ -9263,46 +9286,46 @@
       <c r="O72" s="59">
         <v>12260</v>
       </c>
-      <c r="P72" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q72" s="63">
-        <v>0</v>
-      </c>
-      <c r="R72" s="63">
-        <v>0</v>
-      </c>
-      <c r="S72" s="66">
+      <c r="P72" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q72" s="62">
+        <v>0</v>
+      </c>
+      <c r="R72" s="62">
+        <v>0</v>
+      </c>
+      <c r="S72" s="65">
         <v>20</v>
       </c>
-      <c r="T72" s="66">
+      <c r="T72" s="65">
         <v>16</v>
       </c>
-      <c r="U72" s="64">
-        <v>0</v>
-      </c>
-      <c r="V72" s="63">
-        <v>0</v>
-      </c>
-      <c r="W72" s="63">
-        <v>0</v>
-      </c>
-      <c r="X72" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y72" s="63">
-        <v>0</v>
-      </c>
-      <c r="Z72" s="68">
+      <c r="U72" s="63">
+        <v>0</v>
+      </c>
+      <c r="V72" s="62">
+        <v>0</v>
+      </c>
+      <c r="W72" s="62">
+        <v>0</v>
+      </c>
+      <c r="X72" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y72" s="62">
+        <v>0</v>
+      </c>
+      <c r="Z72" s="67">
         <v>1036</v>
       </c>
-      <c r="AA72" s="68">
+      <c r="AA72" s="67">
         <v>1036</v>
       </c>
-      <c r="AB72" s="71">
-        <v>0</v>
-      </c>
-      <c r="AC72" s="71">
+      <c r="AB72" s="70">
+        <v>0</v>
+      </c>
+      <c r="AC72" s="70">
         <v>0</v>
       </c>
     </row>
@@ -9353,46 +9376,46 @@
       <c r="O73" s="53">
         <v>12260</v>
       </c>
-      <c r="P73" s="63">
-        <v>0</v>
-      </c>
-      <c r="Q73" s="63">
-        <v>0</v>
-      </c>
-      <c r="R73" s="63">
-        <v>0</v>
-      </c>
-      <c r="S73" s="65">
+      <c r="P73" s="62">
+        <v>0</v>
+      </c>
+      <c r="Q73" s="62">
+        <v>0</v>
+      </c>
+      <c r="R73" s="62">
+        <v>0</v>
+      </c>
+      <c r="S73" s="64">
         <v>20</v>
       </c>
-      <c r="T73" s="65">
+      <c r="T73" s="64">
         <v>16</v>
       </c>
-      <c r="U73" s="64">
-        <v>0</v>
-      </c>
-      <c r="V73" s="63">
-        <v>0</v>
-      </c>
-      <c r="W73" s="63">
-        <v>0</v>
-      </c>
-      <c r="X73" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y73" s="63">
-        <v>0</v>
-      </c>
-      <c r="Z73" s="69">
+      <c r="U73" s="63">
+        <v>0</v>
+      </c>
+      <c r="V73" s="62">
+        <v>0</v>
+      </c>
+      <c r="W73" s="62">
+        <v>0</v>
+      </c>
+      <c r="X73" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y73" s="62">
+        <v>0</v>
+      </c>
+      <c r="Z73" s="68">
         <v>2013</v>
       </c>
-      <c r="AA73" s="69">
+      <c r="AA73" s="68">
         <v>2013</v>
       </c>
-      <c r="AB73" s="72">
-        <v>0</v>
-      </c>
-      <c r="AC73" s="72">
+      <c r="AB73" s="71">
+        <v>0</v>
+      </c>
+      <c r="AC73" s="71">
         <v>0</v>
       </c>
     </row>
@@ -9400,4 +9423,133 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{350633A3-3E17-4E1A-B76D-568FECB9C7F8}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="74" t="s">
+        <v>228</v>
+      </c>
+      <c r="B1" s="74"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="72" t="s">
+        <v>217</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C8" si="0">CONCATENATE(A2,B2)</f>
+        <v>ISO20'ARS_ISO</v>
+      </c>
+      <c r="D2" s="73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="72" t="s">
+        <v>230</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>ISO20'_ETOARS_ISO</v>
+      </c>
+      <c r="D3" s="73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="72" t="s">
+        <v>225</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>ISO40'ARS_ISO</v>
+      </c>
+      <c r="D4" s="73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="72" t="s">
+        <v>231</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>ISO40'_ETOARS_ISO</v>
+      </c>
+      <c r="D5" s="73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="72" t="s">
+        <v>226</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>NON ISO25'ARS_NONISO</v>
+      </c>
+      <c r="D6" s="73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="72" t="s">
+        <v>227</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>NON ISO45'ARS_NONISO</v>
+      </c>
+      <c r="D7" s="73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="72" t="s">
+        <v>233</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>NON ISOD45ARS_NONISO</v>
+      </c>
+      <c r="D8" s="73">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>